<commit_message>
frecuencias absolutas y relativas
</commit_message>
<xml_diff>
--- a/Trabajo_práctico_de_evaluación_de_la_Unidad_1/Ingresantes_anonimizado.xlsx
+++ b/Trabajo_práctico_de_evaluación_de_la_Unidad_1/Ingresantes_anonimizado.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\DIPLOMATURA_en_ESTADISTICAS_PUBLICAS-DIPLOMATURA_en_ESTADISTICAS_PUBLICAS\Trabajo_práctico_de_evaluación_de_la_Unidad_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20204041157\Documents\DIPLOMATURA_en_ESTADISTICAS_PUBLICAS\Trabajo_práctico_de_evaluación_de_la_Unidad_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="48">
   <si>
     <t>Género</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Frecuencia relativa</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -11626,23 +11629,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
@@ -11658,7 +11651,7 @@
         <v>237</v>
       </c>
       <c r="C2">
-        <v>0.69096209912536444</v>
+        <v>69.099999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -11669,7 +11662,7 @@
         <v>102</v>
       </c>
       <c r="C3">
-        <v>0.29737609329446058</v>
+        <v>29.74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -11680,7 +11673,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2.9154518950437322E-3</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -11691,7 +11684,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2.9154518950437322E-3</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -11702,7 +11695,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2.9154518950437322E-3</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -11713,73 +11706,98 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2.9154518950437322E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>343</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>132</v>
-      </c>
-      <c r="C11">
-        <v>0.38483965014577259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>95</v>
-      </c>
-      <c r="C12">
-        <v>0.27696793002915449</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="C13">
-        <v>0.14868804664723029</v>
+        <v>38.479999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="C14">
-        <v>0.11661807580174929</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>14.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>25</v>
       </c>
-      <c r="C15">
-        <v>7.2886297376093298E-2</v>
+      <c r="C17">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>343</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>